<commit_message>
test RAG with many model
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10710"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10710" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Case 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>MODEL = gpt-3.5-turbo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>CHUNK SIZE</t>
   </si>
@@ -36,19 +34,80 @@
   </si>
   <si>
     <t>stt</t>
+  </si>
+  <si>
+    <t>MODEL EMBEDDING</t>
+  </si>
+  <si>
+    <t>MODEL GEN ANSWER</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gpt-3.5-turbo</t>
+  </si>
+  <si>
+    <t>gpt-3.5-turbo</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+text-embedding-ada-002 (from openai)</t>
+  </si>
+  <si>
+    <t>phobert(base)</t>
+  </si>
+  <si>
+    <t>mistralai/Mixtral-8x7B-Instruct-v0.1</t>
+  </si>
+  <si>
+    <t>vietnamese sbert</t>
+  </si>
+  <si>
+    <t>phobert(base): unefficient</t>
+  </si>
+  <si>
+    <t>Model name</t>
+  </si>
+  <si>
+    <t>Max length</t>
+  </si>
+  <si>
+    <t>Last_hidden_state shape</t>
+  </si>
+  <si>
+    <t>phobert</t>
+  </si>
+  <si>
+    <t>bartpho</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF050505"/>
+      <name val="Segoe UI Historic"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -71,8 +130,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A2:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -364,28 +430,33 @@
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" customWidth="1"/>
     <col min="6" max="6" width="32.5703125" customWidth="1"/>
+    <col min="10" max="10" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F1" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -395,16 +466,144 @@
       <c r="C3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="C4">
+        <v>200</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1024</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>256</v>
+      </c>
+      <c r="C6">
         <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>256</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="D8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>256</v>
+      </c>
+      <c r="C2">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>1024</v>
+      </c>
+      <c r="C3">
+        <v>1024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test model with wordsgement
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10710" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10710"/>
   </bookViews>
   <sheets>
     <sheet name="Case 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>CHUNK SIZE</t>
   </si>
@@ -58,15 +58,6 @@
 text-embedding-ada-002 (from openai)</t>
   </si>
   <si>
-    <t>phobert(base)</t>
-  </si>
-  <si>
-    <t>mistralai/Mixtral-8x7B-Instruct-v0.1</t>
-  </si>
-  <si>
-    <t>vietnamese sbert</t>
-  </si>
-  <si>
     <t>phobert(base): unefficient</t>
   </si>
   <si>
@@ -83,13 +74,55 @@
   </si>
   <si>
     <t>bartpho</t>
+  </si>
+  <si>
+    <t>bartpho-syllable</t>
+  </si>
+  <si>
+    <t>PADDING</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>POOLING</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>vinai/bartpho-word</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>BAD</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>vinai/phobert-base-v2</t>
+  </si>
+  <si>
+    <t>Preprocess</t>
+  </si>
+  <si>
+    <t>py_vncorenlp.VnCoreNLP (segment)</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Good</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,9 +138,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF050505"/>
-      <name val="Segoe UI Historic"/>
-      <family val="2"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6A9955"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -130,15 +169,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J8"/>
+  <dimension ref="A2:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,13 +474,15 @@
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" customWidth="1"/>
-    <col min="5" max="5" width="42.7109375" customWidth="1"/>
-    <col min="6" max="6" width="32.5703125" customWidth="1"/>
-    <col min="10" max="10" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="66" customWidth="1"/>
+    <col min="5" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="40.28515625" customWidth="1"/>
+    <col min="8" max="8" width="42.7109375" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" customWidth="1"/>
+    <col min="13" max="13" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -447,16 +493,28 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -466,20 +524,20 @@
       <c r="C3">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="M3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -489,67 +547,155 @@
       <c r="C4">
         <v>200</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
         <v>1024</v>
       </c>
-      <c r="C5">
-        <v>100</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
+        <v>1024</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1024</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
         <v>256</v>
       </c>
-      <c r="C6">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7">
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
         <v>256</v>
       </c>
-      <c r="C7">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="D8" s="3" t="s">
-        <v>12</v>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>256</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -562,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,18 +721,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>256</v>
@@ -597,7 +743,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>1024</v>

</xml_diff>

<commit_message>
Research new RAG model
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="37">
   <si>
     <t>CHUNK SIZE</t>
   </si>
   <si>
     <t>CHUNK OVERLAP</t>
-  </si>
-  <si>
-    <t>stt</t>
   </si>
   <si>
     <t>MODEL EMBEDDING</t>
@@ -58,9 +55,6 @@
 text-embedding-ada-002 (from openai)</t>
   </si>
   <si>
-    <t>phobert(base): unefficient</t>
-  </si>
-  <si>
     <t>Model name</t>
   </si>
   <si>
@@ -116,6 +110,38 @@
   </si>
   <si>
     <t>Good</t>
+  </si>
+  <si>
+    <t>File_path_evaluate</t>
+  </si>
+  <si>
+    <t>Chunk method</t>
+  </si>
+  <si>
+    <t>Method_id</t>
+  </si>
+  <si>
+    <t>E:\TrungPhanADVN\Code\LangChain_RAG\scripts\evaluate\embeddings_models\vinai__phobert-base-v2_vncore_segment</t>
+  </si>
+  <si>
+    <t>Recursive(separators=["\r\n\r\n", "\r\n", ".", " ", ""])</t>
+  </si>
+  <si>
+    <t>Recursive(separators=["\r\n\", "\n", ".", " ", ""])</t>
+  </si>
+  <si>
+    <t>E:\TrungPhanADVN\Code\LangChain_RAG\scripts\evaluate\embeddings_models\vinai__bartpho-word_vncore_segment</t>
+  </si>
+  <si>
+    <t>Recursive(separators=["\n\n", "\n", ".", " ", ""])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        doc_splitter = RecursiveCharacterTextSplitter(
+                        chunk_size=LLM_CHUNK_SIZE,
+                        chunk_overlap=LLM_CHUNK_OVERLAP,
+                        add_start_index=True,
+                        separators=[""],
+                    )</t>
   </si>
 </sst>
 </file>
@@ -149,12 +175,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -169,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -181,6 +213,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -463,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M10"/>
+  <dimension ref="A2:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,17 +510,18 @@
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="66" customWidth="1"/>
-    <col min="5" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="40.28515625" customWidth="1"/>
-    <col min="8" max="8" width="42.7109375" customWidth="1"/>
-    <col min="9" max="9" width="32.5703125" customWidth="1"/>
-    <col min="13" max="13" width="30.28515625" customWidth="1"/>
+    <col min="4" max="5" width="66" customWidth="1"/>
+    <col min="6" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="40.28515625" customWidth="1"/>
+    <col min="9" max="9" width="42.7109375" customWidth="1"/>
+    <col min="10" max="10" width="32.5703125" customWidth="1"/>
+    <col min="12" max="12" width="31.42578125" customWidth="1"/>
+    <col min="14" max="14" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -493,28 +530,34 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
         <v>17</v>
       </c>
       <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
-        <v>7</v>
-      </c>
       <c r="J2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -524,20 +567,18 @@
       <c r="C3">
         <v>20</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="I3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -547,28 +588,28 @@
       <c r="C4">
         <v>200</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="H4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
         <v>1024</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
+      <c r="H5" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="I5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -579,19 +620,19 @@
         <v>100</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -602,25 +643,25 @@
         <v>100</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" t="s">
         <v>21</v>
       </c>
-      <c r="I7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -631,53 +672,30 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" t="s">
-        <v>8</v>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>256</v>
-      </c>
-      <c r="C9">
-        <v>20</v>
-      </c>
-      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" t="s">
         <v>27</v>
       </c>
-      <c r="E9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>256</v>
@@ -686,16 +704,243 @@
         <v>20</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="F10" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>21</v>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>256</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>512</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>256</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" t="s">
+        <v>7</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>256</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>512</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>512</v>
+      </c>
+      <c r="C16">
+        <v>50</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>2048</v>
+      </c>
+      <c r="C17">
+        <v>200</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -721,18 +966,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>256</v>
@@ -743,7 +988,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>1024</v>

</xml_diff>